<commit_message>
Agenda updated, README created
</commit_message>
<xml_diff>
--- a/AgendaTable.xlsx
+++ b/AgendaTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liuonline-my.sharepoint.com/personal/erima96_liu_se/Documents/WSps/MDU-RKurs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liuonline-my.sharepoint.com/personal/erima96_liu_se/Documents/WSps/R-WorkshopMDU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{2F70C41A-882A-46EC-9A41-0EFD3AEDF7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA468808-02C2-4AC4-B780-AB615B23518F}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{2F70C41A-882A-46EC-9A41-0EFD3AEDF7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AAA0B196-81AD-4F60-A858-BCF589BAC150}"/>
   <bookViews>
-    <workbookView xWindow="42075" yWindow="4095" windowWidth="28800" windowHeight="15375" xr2:uid="{7B53E4DE-4591-4C0F-A3C6-97E1784E38E1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7B53E4DE-4591-4C0F-A3C6-97E1784E38E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Time</t>
   </si>
@@ -71,37 +71,40 @@
     <t>09:30 - 10:00</t>
   </si>
   <si>
-    <t>Statistics in R 1</t>
-  </si>
-  <si>
     <t>t-test, chi-square, correlation, and assumptionstests etc.</t>
   </si>
   <si>
-    <t>Statistics in R 2</t>
-  </si>
-  <si>
     <t>Regression (linear, logistics, assumptions)</t>
   </si>
   <si>
-    <t>Statistics in R 3</t>
-  </si>
-  <si>
-    <t>Regression continues (may include multilevel)</t>
-  </si>
-  <si>
-    <t>Statistics in R 4</t>
-  </si>
-  <si>
     <t>Reading data, manipulating data, descriptive statistics, etc.</t>
   </si>
   <si>
     <t>15:15 - 16:00</t>
   </si>
   <si>
-    <t>Statistics in R 5</t>
-  </si>
-  <si>
-    <t>Factor Analysis (CFA/SEM, Assumptions)</t>
+    <t>Basic Statistics</t>
+  </si>
+  <si>
+    <t>Regression Modeling 1</t>
+  </si>
+  <si>
+    <t>Regression Modeling 2</t>
+  </si>
+  <si>
+    <t>Regression Modeling 3</t>
+  </si>
+  <si>
+    <t>Factor Analysis</t>
+  </si>
+  <si>
+    <t>e.g., stepwise regression, visualisation, tables</t>
+  </si>
+  <si>
+    <t>Continues (may include multilevel and some ANOVAs)$^a$</t>
+  </si>
+  <si>
+    <t>Confirmatory Factor Analysis and Structural Equation Modeling$^a$</t>
   </si>
 </sst>
 </file>
@@ -456,12 +459,13 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -494,7 +498,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -502,10 +506,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,10 +517,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -524,10 +528,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,21 +539,21 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>